<commit_message>
Update transcription error in swale measurements and update pdf of results
Qgis decided to make a bunch of file changes as well :(
</commit_message>
<xml_diff>
--- a/data/swale-measurements-5-1-24.xlsx
+++ b/data/swale-measurements-5-1-24.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27624"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6BFAAECF-AEE3-4D91-99A1-675C4576F069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{85D7B9FD-98E7-4AB6-A702-114C3B7AF419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>Center Depth</t>
+  </si>
+  <si>
+    <t>Left Wetted</t>
+  </si>
+  <si>
+    <t>Right Wetted</t>
   </si>
   <si>
     <t>Total Length</t>
@@ -463,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -477,14 +483,14 @@
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="8" max="10" width="14.85546875" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" customWidth="1"/>
-    <col min="12" max="13" width="14.85546875" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" customWidth="1"/>
-    <col min="15" max="15" width="14.5703125" customWidth="1"/>
+    <col min="8" max="12" width="14.85546875" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" customWidth="1"/>
+    <col min="14" max="15" width="14.85546875" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" customWidth="1"/>
+    <col min="17" max="17" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -530,10 +536,16 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>36</v>
@@ -557,9 +569,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>48</v>
@@ -583,9 +595,9 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>64</v>
@@ -609,12 +621,13 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B5">
-        <v>6.5</v>
+        <f xml:space="preserve"> 6.5 * 12</f>
+        <v>78</v>
       </c>
       <c r="C5">
         <v>20</v>
@@ -635,9 +648,9 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <f>8*12</f>
@@ -662,9 +675,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B7">
         <f>6*12</f>
@@ -689,41 +702,41 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8">
+        <v>17</v>
+      </c>
+      <c r="K8">
         <v>160</v>
       </c>
-      <c r="J8">
+      <c r="L8">
         <f>AVERAGE(B2:B7)/12</f>
-        <v>4.479166666666667</v>
-      </c>
-      <c r="K8">
+        <v>5.4722222222222223</v>
+      </c>
+      <c r="M8">
         <f>AVERAGE(C2:C7)/12</f>
         <v>1.5138888888888891</v>
       </c>
-      <c r="L8" s="2">
+      <c r="N8" s="2">
         <f>AVERAGE(D2:D7)/AVERAGE(E2:E7)</f>
         <v>0.50485436893203872</v>
       </c>
-      <c r="M8">
+      <c r="O8">
         <f>AVERAGE(F2:F7)/AVERAGE(G2:G7)</f>
         <v>0.28125</v>
       </c>
-      <c r="N8">
-        <f>AVERAGE(L8,M8)/12</f>
+      <c r="P8">
+        <f>AVERAGE(N8,O8)/12</f>
         <v>3.2754348705501611E-2</v>
       </c>
-      <c r="O8">
+      <c r="Q8">
         <f>AVERAGE(H2:H7)/12</f>
         <v>0.80555555555555547</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>48</v>
@@ -747,9 +760,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>80</v>
@@ -770,12 +783,12 @@
         <v>40</v>
       </c>
       <c r="H10">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B11">
         <v>48</v>
@@ -799,9 +812,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>36</v>
@@ -825,36 +838,36 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13">
+        <v>18</v>
+      </c>
+      <c r="K13">
         <v>58</v>
       </c>
-      <c r="J13">
+      <c r="L13">
         <f>AVERAGE(B9:B12)/12</f>
         <v>4.416666666666667</v>
       </c>
-      <c r="K13">
+      <c r="M13">
         <f>AVERAGE(C9:C12)/12</f>
         <v>1.5625</v>
       </c>
-      <c r="L13" s="2">
+      <c r="N13" s="2">
         <f>AVERAGE(D7:D12)/AVERAGE(D9:E12)/12</f>
         <v>4.9087893864013271E-2</v>
       </c>
-      <c r="M13">
+      <c r="O13">
         <f>AVERAGE(F9:F12)/AVERAGE(G9:G12)</f>
         <v>0.29113924050632911</v>
       </c>
-      <c r="N13">
-        <f>AVERAGE(L13,M13)/12</f>
+      <c r="P13">
+        <f>AVERAGE(N13,O13)/12</f>
         <v>1.4176130598764264E-2</v>
       </c>
-      <c r="O13">
+      <c r="Q13">
         <f>AVERAGE(H9:H12)/12</f>
-        <v>1.3125</v>
+        <v>0.46875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>